<commit_message>
Updates the HostView wireframes
Changed the "Cancel" button in ifrNewTicket/NewTicket.php to "Back"

changed ifrSelectedTable/SelectedTable.php to show multiple servers. Each server now has a remove button beside them
</commit_message>
<xml_diff>
--- a/Documentation/HostView/HostViewWireframes.xlsx
+++ b/Documentation/HostView/HostViewWireframes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\HostView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A68BB5-3510-46F6-AC76-52885B09DB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF01398-E0FE-4D7C-BB11-E0A05E784CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E23D887-9FAB-4E8E-922D-058863E57D09}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{4E23D887-9FAB-4E8E-922D-058863E57D09}"/>
   </bookViews>
   <sheets>
     <sheet name="HostView.php" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>server</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Wait Times</t>
-  </si>
-  <si>
-    <t>▼</t>
   </si>
   <si>
     <t>Upper</t>
@@ -317,33 +314,12 @@
     <t>Assigned Ticket</t>
   </si>
   <si>
-    <t>Seated</t>
-  </si>
-  <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
-    <t>Assigned</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Status</t>
   </si>
   <si>
     <t>Selected Ticket: 7</t>
   </si>
   <si>
-    <t>Assign Server</t>
-  </si>
-  <si>
-    <t>Assign Ticket</t>
-  </si>
-  <si>
-    <t>Needs more room to allow for 3 servers tops</t>
-  </si>
-  <si>
-    <t>Disabled</t>
-  </si>
-  <si>
     <t>Assign ticket won't be visible if status is Seated or Disabled</t>
   </si>
   <si>
@@ -354,12 +330,6 @@
   </si>
   <si>
     <t>around their tables?</t>
-  </si>
-  <si>
-    <t>Clicking on a table here will populate ifrSelectedTable</t>
-  </si>
-  <si>
-    <t>and ifrTicket if there is a ticked assigned to it</t>
   </si>
   <si>
     <t>Only correct states should be available here</t>
@@ -637,9 +607,6 @@
     </r>
   </si>
   <si>
-    <t>HostView can enable/disable Assign Server/Ticket variables</t>
-  </si>
-  <si>
     <r>
       <t>ORDER BY timeRequested, timeReserved;</t>
     </r>
@@ -680,35 +647,158 @@
     <t>New Ticket</t>
   </si>
   <si>
-    <t>Party Name</t>
-  </si>
-  <si>
-    <t>Party Size</t>
-  </si>
-  <si>
-    <t>Time Requested</t>
-  </si>
-  <si>
-    <t>horton</t>
-  </si>
-  <si>
-    <t>Create Ticket</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
-  <si>
-    <t>NewTicket.php</t>
-  </si>
-  <si>
     <t>Create ticket button submits back to NewTicket.php</t>
   </si>
   <si>
-    <t>Cancel button routes to WaitList.php</t>
-  </si>
-  <si>
-    <r>
-      <t>Add button links to another page…</t>
+    <r>
+      <t xml:space="preserve">PHP code should check for sumbitted data and use the SQL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CALL createTicket(nickname, partySize, timeRequested, @newTicketNumber);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Must have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>include 'Resources/php/display.php';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> immedately before the closing &lt;/form&gt; tag</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If any of the 3 inputs are changed, they must call one of: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">setVar("lowerVal", THE_LOWER_VALUE);  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">setVar("upperVal", THE_UPPER_VALUE); </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">and finally call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>updateDisplay();</t>
+    </r>
+  </si>
+  <si>
+    <t>setVar("minsAgoVal", MINSAGO_VALUE);</t>
+  </si>
+  <si>
+    <t>See displayInterface.php</t>
+  </si>
+  <si>
+    <t>This will force a refresh and retain the</t>
+  </si>
+  <si>
+    <t>values of lower, upper, and mins ago</t>
+  </si>
+  <si>
+    <t>Restaurant diagram with clickable tables displayed here</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>HostView will have the ability to inject hidden inputs into this php.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This php should directly insert records into the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TableLog</t>
+    </r>
+  </si>
+  <si>
+    <t>$_POST['employeeId'], $_POST['ticketId'].</t>
+  </si>
+  <si>
+    <t>It should look for $_POST['tableId'], $_POST['action'], $_POST['authorizationId'].</t>
+  </si>
+  <si>
+    <t>There must also be a combination of 1 or both of:</t>
+  </si>
+  <si>
+    <t>Note: inserting into the table log may throw SQL errors</t>
+  </si>
+  <si>
+    <t>Handle them by displaying the human readable error</t>
+  </si>
+  <si>
+    <t>to the Host with an alert or popup</t>
+  </si>
+  <si>
+    <t>If only the  $_POST['tableId'] is found, just populate the html.</t>
+  </si>
+  <si>
+    <t>If  $_POST['tableId'] isn't set, display "No Table Selected"</t>
+  </si>
+  <si>
+    <t>Clicking on a table here will populate ifrSelectedTable
+and ifrTicket if there is a ticked assigned to it</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>This is a fixed list of table stauses</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>ifrRestaurantLayout</t>
+  </si>
+  <si>
+    <t>ifrWaitList : mode 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Add button links to</t>
     </r>
     <r>
       <rPr>
@@ -724,7 +814,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">PHP code should check for sumbitted data and use the SQL </t>
+      <t xml:space="preserve">Back button links to </t>
     </r>
     <r>
       <rPr>
@@ -735,123 +825,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CALL createTicket(nickname, partySize, timeRequested, @newTicketNumber);</t>
-    </r>
-  </si>
-  <si>
-    <t>A better name would be "Back"…. Host may want to create several new tickets and then go "Back" to WaitList.php</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Must have </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>include 'Resources/php/display.php';</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> immedately before the closing &lt;/form&gt; tag</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">If any of the 3 inputs are changed, they must call one of: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">setVar("lowerVal", THE_LOWER_VALUE);  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">setVar("upperVal", THE_UPPER_VALUE); </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">and finally call </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>updateDisplay();</t>
-    </r>
-  </si>
-  <si>
-    <t>setVar("minsAgoVal", MINSAGO_VALUE);</t>
-  </si>
-  <si>
-    <t>See displayInterface.php</t>
-  </si>
-  <si>
-    <t>This will force a refresh and retain the</t>
-  </si>
-  <si>
-    <t>values of lower, upper, and mins ago</t>
-  </si>
-  <si>
-    <t>Restaurant diagram with clickable tables displayed here</t>
-  </si>
-  <si>
-    <t>Javascript</t>
-  </si>
-  <si>
-    <t>HostView will have the ability to inject hidden inputs into this php.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This php should directly insert records into the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TableLog</t>
-    </r>
-  </si>
-  <si>
-    <t>$_POST['employeeId'], $_POST['ticketId'].</t>
-  </si>
-  <si>
-    <t>It should look for $_POST['tableId'], $_POST['action'], $_POST['authorizationId'].</t>
-  </si>
-  <si>
-    <t>There must also be a combination of 1 or both of:</t>
-  </si>
-  <si>
-    <t>Note: inserting into the table log may throw SQL errors</t>
-  </si>
-  <si>
-    <t>Handle them by displaying the human readable error</t>
-  </si>
-  <si>
-    <t>to the Host with an alert or popup</t>
-  </si>
-  <si>
-    <t>If only the  $_POST['tableId'] is found, just populate the html.</t>
-  </si>
-  <si>
-    <t>If  $_POST['tableId'] isn't set, display "No Table Selected"</t>
+      <t>WaitList.php</t>
+    </r>
+  </si>
+  <si>
+    <t>Host may want to create several new tickets and then go "Back" to WaitList.php</t>
+  </si>
+  <si>
+    <t>Pressing back will cancel any entered data and not be submitted. Do we need to alert the Host for this?</t>
   </si>
 </sst>
 </file>
@@ -984,7 +965,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1174,19 +1155,6 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1236,19 +1204,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1312,18 +1267,59 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1340,9 +1336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1355,11 +1348,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1370,19 +1360,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1391,40 +1381,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1436,33 +1405,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1478,13 +1420,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1492,31 +1430,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1525,28 +1448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1563,9 +1465,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1573,56 +1473,150 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1652,9 +1646,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1713,9 +1707,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>120650</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1774,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1828,23 +1822,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61F5CA7-739C-4EDD-3701-503F4FE5230D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B53F0FD-43EE-6CA4-9417-8524C87E85AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1867,191 +1861,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10125075" y="1597025"/>
-          <a:ext cx="615950" cy="203200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F688C5C7-F1A1-AE76-FFFB-74B4ADFA380B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10125075" y="1949450"/>
-          <a:ext cx="615950" cy="203200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B53F0FD-43EE-6CA4-9417-8524C87E85AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9093200" y="2276475"/>
+          <a:off x="9093200" y="2314575"/>
           <a:ext cx="1727200" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D4B97F-95A3-2265-8CA0-68E1C7F75B65}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="11407775" y="638175"/>
-          <a:ext cx="946150" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2097,7 +1908,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2141,8 +1952,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>105311</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>149761</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2158,7 +1969,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2196,14 +2007,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2219,7 +2030,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2233,69 +2044,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="161925" y="10277475"/>
-          <a:ext cx="866775" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A071EF99-74B4-2B7B-748E-55A335C13967}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1143000" y="10277475"/>
-          <a:ext cx="863600" cy="190500"/>
+          <a:off x="158750" y="10248900"/>
+          <a:ext cx="857250" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2316,32 +2066,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CBFB0C8-F47B-122D-4579-5FD4F7786AA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA44FBB5-9EB2-136B-8920-710CBB8A1534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8162925" y="2381250"/>
-          <a:ext cx="685800" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="2162175" y="2381250"/>
+          <a:ext cx="6553200" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2365,6 +2115,403 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{823C2812-A9C8-1439-E921-FFB6FCB8219D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5353050" y="2390775"/>
+          <a:ext cx="2578100" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5371C66-374B-F09E-EA76-C073C7D06400}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2162175" y="2400300"/>
+          <a:ext cx="2057400" cy="1847850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AF10E8-39E5-74FB-4E1A-50C1AD5AEBA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10086975" y="1628775"/>
+          <a:ext cx="733425" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D1B57B-73BD-44A7-314A-D47AC56C1EE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10086975" y="2057400"/>
+          <a:ext cx="733425" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>14942</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>343647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>82177</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F84E1FB-3BB1-2310-7F96-5B14DD7835B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7664824" y="4086412"/>
+          <a:ext cx="1232647" cy="814294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>939800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>317500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A5AFFA-0658-182A-2AC6-9CCFF55A2C45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10966450" y="1098550"/>
+          <a:ext cx="939800" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFC63121-207C-8083-FEBC-1B6605EAFF4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1117600" y="10248900"/>
+          <a:ext cx="863600" cy="196850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2552,67 +2699,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938194DB-6411-2D7A-C9EB-788F084AC815}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="47625" y="4171950"/>
-          <a:ext cx="1933575" cy="1524000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2729,6 +2815,67 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8DBC7CF-054C-9199-D080-8598EA0C7546}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="25400" y="4127500"/>
+          <a:ext cx="1930400" cy="1549400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2803,22 +2950,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E32DE402-D6BD-0BDD-EA8A-9F4B403236C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69026A75-106B-21AD-BE07-AB2082432ECC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2841,7 +2988,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="28575" y="28575"/>
+          <a:off x="47625" y="47625"/>
           <a:ext cx="1933575" cy="2438400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3164,10 +3311,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BB51"/>
+  <dimension ref="B1:BH59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18:T29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3189,7 +3336,7 @@
     <col min="26" max="27" width="2.90625" style="1" customWidth="1"/>
     <col min="28" max="28" width="0.90625" style="1" customWidth="1"/>
     <col min="29" max="29" width="1.453125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.81640625" style="1" customWidth="1"/>
     <col min="31" max="31" width="2.7265625" style="1" customWidth="1"/>
     <col min="32" max="32" width="8.7265625" style="1"/>
     <col min="33" max="33" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
@@ -3201,43 +3348,45 @@
     <col min="52" max="52" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="0.453125" style="1" hidden="1" customWidth="1"/>
     <col min="54" max="56" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="57" max="16384" width="8.7265625" style="1"/>
+    <col min="57" max="59" width="8.7265625" style="1"/>
+    <col min="60" max="60" width="1.7265625" style="1" customWidth="1"/>
+    <col min="61" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="34" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:32" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:32" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="J3" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="46"/>
-      <c r="V3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="25"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="85"/>
+      <c r="J3" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="94"/>
+      <c r="V3" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="84"/>
+      <c r="AA3" s="84"/>
+      <c r="AB3" s="85"/>
     </row>
     <row r="4" spans="2:32" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
@@ -3248,16 +3397,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="6"/>
       <c r="V4" s="2"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -3268,298 +3408,244 @@
     </row>
     <row r="5" spans="2:32" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="J5" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="68"/>
       <c r="V5" s="5"/>
-      <c r="W5" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="59"/>
-      <c r="Z5" s="59"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="7"/>
+      <c r="W5" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="82"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="6"/>
       <c r="AF5" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14">
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12">
         <v>5</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <v>3</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="68"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="67"/>
-      <c r="AB6" s="7"/>
-      <c r="AF6" s="78" t="s">
-        <v>54</v>
+      <c r="W6" s="39"/>
+      <c r="X6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="6"/>
+      <c r="AF6" s="46" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12">
         <v>5</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>2</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="6"/>
       <c r="J7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="T7" s="6"/>
       <c r="V7" s="5"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="7"/>
-      <c r="AD7" s="1" t="s">
-        <v>45</v>
+      <c r="W7" s="41"/>
+      <c r="X7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="6"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="111" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF7" s="21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12">
         <v>16</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>3</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="6"/>
       <c r="J8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="T8" s="6"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="7"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="109" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12">
         <v>19</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <v>4</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="7"/>
+      <c r="T9" s="6"/>
       <c r="V9" s="5"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="71"/>
-      <c r="Z9" s="71"/>
-      <c r="AA9" s="72"/>
-      <c r="AB9" s="7"/>
-      <c r="AD9" s="1" t="s">
-        <v>47</v>
+      <c r="W9" s="43"/>
+      <c r="Y9" s="44"/>
+      <c r="Z9" s="44"/>
+      <c r="AA9" s="45"/>
+      <c r="AB9" s="6"/>
+      <c r="AD9" s="109" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="7"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="7"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="6"/>
+      <c r="J10" s="37"/>
+      <c r="T10" s="6"/>
       <c r="V10" s="5"/>
-      <c r="W10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="7"/>
-      <c r="AD10" s="1" t="s">
-        <v>48</v>
+      <c r="W10" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="96"/>
+      <c r="Y10" s="96"/>
+      <c r="Z10" s="96"/>
+      <c r="AA10" s="96"/>
+      <c r="AB10" s="6"/>
+      <c r="AD10" s="46" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:32" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="7"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="J11" s="37"/>
+      <c r="T11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="9"/>
     </row>
     <row r="12" spans="2:32" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="7"/>
+      <c r="T12" s="6"/>
     </row>
     <row r="13" spans="2:32" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="56"/>
-      <c r="V13" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="25"/>
-    </row>
-    <row r="14" spans="2:32" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="85"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="36"/>
+      <c r="V13" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="W13" s="84"/>
+      <c r="X13" s="84"/>
+      <c r="Y13" s="84"/>
+      <c r="Z13" s="84"/>
+      <c r="AA13" s="84"/>
+      <c r="AB13" s="85"/>
+    </row>
+    <row r="14" spans="2:32" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -3567,674 +3653,554 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="56"/>
-      <c r="V14" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="62"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="36"/>
+      <c r="V14" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="W14" s="87"/>
+      <c r="X14" s="87"/>
+      <c r="Y14" s="87"/>
+      <c r="Z14" s="87"/>
+      <c r="AA14" s="87"/>
+      <c r="AB14" s="88"/>
     </row>
     <row r="15" spans="2:32" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="16" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="J15" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="92"/>
-      <c r="V15" s="63"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="64"/>
-    </row>
-    <row r="16" spans="2:32" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="6"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="100"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="58"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="67"/>
+      <c r="X15" s="67"/>
+      <c r="Y15" s="67"/>
+      <c r="Z15" s="67"/>
+      <c r="AA15" s="67"/>
+      <c r="AB15" s="68"/>
+    </row>
+    <row r="16" spans="2:32" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="19">
+      <c r="C16" s="19"/>
+      <c r="D16" s="17">
         <v>0.69097222222222221</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="22">
+      <c r="F16" s="12"/>
+      <c r="G16" s="20">
         <v>7</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="J16" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="92"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="64"/>
+      <c r="H16" s="6"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="58"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="67"/>
+      <c r="X16" s="67"/>
+      <c r="Y16" s="67"/>
+      <c r="Z16" s="67"/>
+      <c r="AA16" s="67"/>
+      <c r="AB16" s="68"/>
     </row>
     <row r="17" spans="2:54" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="19">
+      <c r="C17" s="11"/>
+      <c r="D17" s="17">
         <v>0.69097222222222221</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="22">
+      <c r="F17" s="12"/>
+      <c r="G17" s="20">
         <v>2</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="6"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="7"/>
-      <c r="V17" s="63"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="64"/>
+      <c r="T17" s="6"/>
+      <c r="V17" s="66"/>
+      <c r="W17" s="67"/>
+      <c r="X17" s="67"/>
+      <c r="Y17" s="67"/>
+      <c r="Z17" s="67"/>
+      <c r="AA17" s="67"/>
+      <c r="AB17" s="68"/>
     </row>
     <row r="18" spans="2:54" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="19">
+      <c r="C18" s="11"/>
+      <c r="D18" s="17">
         <v>0.69444444444444453</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="22">
+      <c r="F18" s="12"/>
+      <c r="G18" s="20">
         <v>1</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="J18" s="108" t="s">
-        <v>94</v>
-      </c>
-      <c r="K18" s="109"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109"/>
-      <c r="N18" s="109"/>
-      <c r="O18" s="109"/>
-      <c r="P18" s="109"/>
-      <c r="Q18" s="109"/>
-      <c r="R18" s="109"/>
-      <c r="S18" s="109"/>
-      <c r="T18" s="110"/>
-      <c r="V18" s="63"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="64"/>
+      <c r="H18" s="6"/>
+      <c r="J18" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="74"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="67"/>
+      <c r="Y18" s="67"/>
+      <c r="Z18" s="67"/>
+      <c r="AA18" s="67"/>
+      <c r="AB18" s="68"/>
     </row>
     <row r="19" spans="2:54" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="19">
+      <c r="C19" s="11"/>
+      <c r="D19" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="22">
+      <c r="F19" s="12"/>
+      <c r="G19" s="20">
         <v>3</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="109"/>
-      <c r="O19" s="109"/>
-      <c r="P19" s="109"/>
-      <c r="Q19" s="109"/>
-      <c r="R19" s="109"/>
-      <c r="S19" s="109"/>
-      <c r="T19" s="110"/>
-      <c r="V19" s="63"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="64"/>
+      <c r="H19" s="6"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73"/>
+      <c r="S19" s="73"/>
+      <c r="T19" s="74"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="67"/>
+      <c r="X19" s="67"/>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="67"/>
+      <c r="AA19" s="67"/>
+      <c r="AB19" s="68"/>
     </row>
     <row r="20" spans="2:54" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="7"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
-      <c r="N20" s="109"/>
-      <c r="O20" s="109"/>
-      <c r="P20" s="109"/>
-      <c r="Q20" s="109"/>
-      <c r="R20" s="109"/>
-      <c r="S20" s="109"/>
-      <c r="T20" s="110"/>
-      <c r="V20" s="63"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="64"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="6"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="74"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
+      <c r="Y20" s="67"/>
+      <c r="Z20" s="67"/>
+      <c r="AA20" s="67"/>
+      <c r="AB20" s="68"/>
     </row>
     <row r="21" spans="2:54" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="7"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="109"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="109"/>
-      <c r="S21" s="109"/>
-      <c r="T21" s="110"/>
-      <c r="V21" s="63"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="64"/>
-      <c r="AQ21" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS21" s="32" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="6"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="73"/>
+      <c r="R21" s="73"/>
+      <c r="S21" s="73"/>
+      <c r="T21" s="74"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="67"/>
+      <c r="X21" s="67"/>
+      <c r="Y21" s="67"/>
+      <c r="Z21" s="67"/>
+      <c r="AA21" s="67"/>
+      <c r="AB21" s="68"/>
+      <c r="AQ21" s="24" t="s">
         <v>19</v>
       </c>
+      <c r="AS21" s="24" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="2:54" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="8"/>
-      <c r="C22" s="33" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="10"/>
-      <c r="J22" s="108"/>
-      <c r="K22" s="109"/>
-      <c r="L22" s="109"/>
-      <c r="M22" s="109"/>
-      <c r="N22" s="109"/>
-      <c r="O22" s="109"/>
-      <c r="P22" s="109"/>
-      <c r="Q22" s="109"/>
-      <c r="R22" s="109"/>
-      <c r="S22" s="109"/>
-      <c r="T22" s="110"/>
-      <c r="V22" s="63"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="64"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="9"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73"/>
+      <c r="S22" s="73"/>
+      <c r="T22" s="74"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="67"/>
+      <c r="X22" s="67"/>
+      <c r="Y22" s="67"/>
+      <c r="Z22" s="67"/>
+      <c r="AA22" s="67"/>
+      <c r="AB22" s="68"/>
     </row>
     <row r="23" spans="2:54" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J23" s="108"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="109"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="109"/>
-      <c r="T23" s="110"/>
-      <c r="V23" s="63"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="64"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="73"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="73"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="74"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="67"/>
+      <c r="X23" s="67"/>
+      <c r="Y23" s="67"/>
+      <c r="Z23" s="67"/>
+      <c r="AA23" s="67"/>
+      <c r="AB23" s="68"/>
     </row>
     <row r="24" spans="2:54" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25"/>
-      <c r="J24" s="108"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
-      <c r="O24" s="109"/>
-      <c r="P24" s="109"/>
-      <c r="Q24" s="109"/>
-      <c r="R24" s="109"/>
-      <c r="S24" s="109"/>
-      <c r="T24" s="110"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="64"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="74"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="67"/>
+      <c r="X24" s="67"/>
+      <c r="Y24" s="67"/>
+      <c r="Z24" s="67"/>
+      <c r="AA24" s="67"/>
+      <c r="AB24" s="68"/>
     </row>
     <row r="25" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7"/>
-      <c r="J25" s="108"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="109"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="109"/>
-      <c r="S25" s="109"/>
-      <c r="T25" s="110"/>
-      <c r="V25" s="63"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="64"/>
+      <c r="H25" s="6"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="74"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="67"/>
+      <c r="X25" s="67"/>
+      <c r="Y25" s="67"/>
+      <c r="Z25" s="67"/>
+      <c r="AA25" s="67"/>
+      <c r="AB25" s="68"/>
     </row>
     <row r="26" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
-      <c r="O26" s="109"/>
-      <c r="P26" s="109"/>
-      <c r="Q26" s="109"/>
-      <c r="R26" s="109"/>
-      <c r="S26" s="109"/>
-      <c r="T26" s="110"/>
-      <c r="V26" s="63"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="64"/>
-      <c r="AQ26" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR26" s="36"/>
-      <c r="AS26" s="36" t="s">
+      <c r="H26" s="6"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="73"/>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="74"/>
+      <c r="V26" s="66"/>
+      <c r="W26" s="67"/>
+      <c r="X26" s="67"/>
+      <c r="Y26" s="67"/>
+      <c r="Z26" s="67"/>
+      <c r="AA26" s="67"/>
+      <c r="AB26" s="68"/>
+      <c r="AQ26" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AT26" s="36"/>
-      <c r="AU26" s="36" t="s">
-        <v>32</v>
+      <c r="AR26" s="27"/>
+      <c r="AS26" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT26" s="27"/>
+      <c r="AU26" s="27" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="109"/>
-      <c r="Q27" s="109"/>
-      <c r="R27" s="109"/>
-      <c r="S27" s="109"/>
-      <c r="T27" s="110"/>
-      <c r="V27" s="63"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="64"/>
-      <c r="AX27" s="35">
+      <c r="H27" s="6"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="73"/>
+      <c r="T27" s="74"/>
+      <c r="V27" s="66"/>
+      <c r="W27" s="67"/>
+      <c r="X27" s="67"/>
+      <c r="Y27" s="67"/>
+      <c r="Z27" s="67"/>
+      <c r="AA27" s="67"/>
+      <c r="AB27" s="68"/>
+      <c r="AX27" s="26">
         <v>2</v>
       </c>
-      <c r="AY27" s="37"/>
-      <c r="AZ27" s="35">
+      <c r="AY27" s="28"/>
+      <c r="AZ27" s="26">
         <v>5</v>
       </c>
-      <c r="BA27" s="37"/>
-      <c r="BB27" s="35">
+      <c r="BA27" s="28"/>
+      <c r="BB27" s="26">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:54" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="J28" s="108"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="109"/>
-      <c r="O28" s="109"/>
-      <c r="P28" s="109"/>
-      <c r="Q28" s="109"/>
-      <c r="R28" s="109"/>
-      <c r="S28" s="109"/>
-      <c r="T28" s="110"/>
-      <c r="V28" s="63"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="64"/>
+      <c r="H28" s="6"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="73"/>
+      <c r="Q28" s="73"/>
+      <c r="R28" s="73"/>
+      <c r="S28" s="73"/>
+      <c r="T28" s="74"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="67"/>
+      <c r="Y28" s="67"/>
+      <c r="Z28" s="67"/>
+      <c r="AA28" s="67"/>
+      <c r="AB28" s="68"/>
     </row>
     <row r="29" spans="2:54" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="43"/>
-      <c r="J29" s="111"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="112"/>
-      <c r="M29" s="112"/>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="112"/>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="112"/>
-      <c r="S29" s="112"/>
-      <c r="T29" s="113"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="33"/>
-      <c r="Y29" s="33"/>
-      <c r="Z29" s="33"/>
-      <c r="AA29" s="33"/>
-      <c r="AB29" s="43"/>
-      <c r="AX29" s="39" t="s">
+      <c r="B29" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="AY29" s="40"/>
-      <c r="AZ29" s="40"/>
-      <c r="BA29" s="40"/>
-      <c r="BB29" s="41"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="76"/>
+      <c r="P29" s="76"/>
+      <c r="Q29" s="76"/>
+      <c r="R29" s="76"/>
+      <c r="S29" s="76"/>
+      <c r="T29" s="77"/>
+      <c r="V29" s="69"/>
+      <c r="W29" s="70"/>
+      <c r="X29" s="70"/>
+      <c r="Y29" s="70"/>
+      <c r="Z29" s="70"/>
+      <c r="AA29" s="70"/>
+      <c r="AB29" s="71"/>
+      <c r="AX29" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY29" s="90"/>
+      <c r="AZ29" s="90"/>
+      <c r="BA29" s="90"/>
+      <c r="BB29" s="91"/>
     </row>
     <row r="30" spans="2:54" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="2:54" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="AD32" s="28" t="s">
+    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="2:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="80"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="5"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="5"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="5"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="5"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:8" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="5"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="68"/>
+    </row>
+    <row r="47" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="69"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="71"/>
+    </row>
+    <row r="55" spans="59:60" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="56" spans="59:60" x14ac:dyDescent="0.35">
+      <c r="BG56" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="AG32" s="35">
+      <c r="BH56" s="107" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="59:60" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BG57" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH57" s="108" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="59:60" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BG59" s="110">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="AD34" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE34" s="74" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:35" hidden="1" x14ac:dyDescent="0.35">
-      <c r="AD35" s="75" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="2:35" hidden="1" x14ac:dyDescent="0.35">
-      <c r="AD36" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI36" s="73" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="AD37" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG37" s="73" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="2:35" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="2:35" ht="23.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="93"/>
-      <c r="H40" s="94"/>
-    </row>
-    <row r="41" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="7"/>
-      <c r="M42" s="95" t="s">
-        <v>73</v>
-      </c>
-      <c r="N42" s="95"/>
-      <c r="O42" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="P42" s="97"/>
-    </row>
-    <row r="43" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="7"/>
-      <c r="M43" s="95" t="s">
-        <v>74</v>
-      </c>
-      <c r="N43" s="95"/>
-      <c r="O43" s="96">
-        <v>7</v>
-      </c>
-      <c r="P43" s="97"/>
-    </row>
-    <row r="44" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="5"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="7"/>
-      <c r="M44" s="95" t="s">
-        <v>75</v>
-      </c>
-      <c r="N44" s="95"/>
-      <c r="O44" s="98">
-        <v>0.74305555555555547</v>
-      </c>
-      <c r="P44" s="97"/>
-    </row>
-    <row r="45" spans="2:35" ht="8.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="2:35" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="64"/>
-      <c r="AG46" s="37"/>
-    </row>
-    <row r="47" spans="2:35" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="42"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="43"/>
-      <c r="AG47" s="99" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="2:35" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="33:33" hidden="1" x14ac:dyDescent="0.35">
-      <c r="AG49" s="99" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="33:33" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="33:33" hidden="1" x14ac:dyDescent="0.35"/>
+      <c r="BH59" s="108" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D6:G9">
     <sortCondition ref="F6:F9"/>
   </sortState>
-  <mergeCells count="24">
-    <mergeCell ref="B46:H47"/>
-    <mergeCell ref="J18:T29"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="W5:AA5"/>
-    <mergeCell ref="V13:AB13"/>
-    <mergeCell ref="V14:AB29"/>
-    <mergeCell ref="J15:T15"/>
-    <mergeCell ref="J16:T16"/>
+  <mergeCells count="18">
     <mergeCell ref="AX29:BB29"/>
     <mergeCell ref="B29:H29"/>
     <mergeCell ref="J3:T3"/>
@@ -4245,6 +4211,14 @@
     <mergeCell ref="B24:H24"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B13:H13"/>
+    <mergeCell ref="L15:R16"/>
+    <mergeCell ref="J5:T6"/>
+    <mergeCell ref="W5:AA5"/>
+    <mergeCell ref="V13:AB13"/>
+    <mergeCell ref="V14:AB29"/>
+    <mergeCell ref="B46:H47"/>
+    <mergeCell ref="J18:T29"/>
+    <mergeCell ref="B40:H40"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -4267,92 +4241,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="D1" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="6"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="6" t="s">
-        <v>30</v>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="6" t="s">
-        <v>27</v>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="6"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="4:15" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="6" t="s">
-        <v>26</v>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D7" s="6" t="s">
-        <v>64</v>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D8" s="6"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D9" s="6" t="s">
-        <v>29</v>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D10" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
+      <c r="D10" s="34" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D11" s="90" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
+      <c r="D11" s="56" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D14" s="101" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
+      <c r="D14" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
     </row>
     <row r="15" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D15" s="101" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="102"/>
+      <c r="D15" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4363,10 +4329,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645F9BC3-FD70-45E7-BF31-A2F0860E127B}">
-  <dimension ref="D1:N30"/>
+  <dimension ref="D1:N31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4375,130 +4341,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D1" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
+      <c r="D1" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="4" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="D5" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D6" s="88" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="D6" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D7" s="82" t="s">
-        <v>61</v>
+      <c r="D7" s="50" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
+      <c r="D9" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D10" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
+      <c r="D10" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D11" s="81" t="s">
-        <v>71</v>
+      <c r="D11" s="49" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D13" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="86"/>
+      <c r="D13" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D14" s="82" t="s">
-        <v>60</v>
+      <c r="D14" s="50" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D15" s="82" t="s">
-        <v>58</v>
+      <c r="D15" s="50" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D16" s="82" t="s">
-        <v>62</v>
+      <c r="D16" s="50" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D18" s="82" t="s">
-        <v>82</v>
+      <c r="D18" s="50" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
-        <v>84</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4522,211 +4486,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
+      <c r="D1" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D2" s="100" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="D2" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D4" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="104"/>
+      <c r="D4" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="62"/>
       <c r="J4" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D5" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="91"/>
+      <c r="D5" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="57"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D6" s="81" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="91"/>
+      <c r="D6" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="57"/>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D7" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="91"/>
+      <c r="D7" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="57"/>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D8" s="82"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="91"/>
+      <c r="D8" s="50"/>
+      <c r="I8" s="57"/>
       <c r="J8" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="107"/>
+      <c r="D9" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D14" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
+      <c r="D14" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="98"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4742,7 +4690,7 @@
   <dimension ref="D1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4753,60 +4701,60 @@
   <sheetData>
     <row r="1" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D3" s="83" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="86"/>
+      <c r="D3" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D4" s="88" t="s">
-        <v>99</v>
+      <c r="D4" s="55" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D5" s="82" t="s">
-        <v>100</v>
+      <c r="D5" s="50" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D6" s="82"/>
+      <c r="D6" s="50"/>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D8" s="82" t="s">
-        <v>101</v>
+      <c r="D8" s="50" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D9" s="82" t="s">
-        <v>102</v>
+      <c r="D9" s="50" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D10" s="82" t="s">
-        <v>103</v>
+      <c r="D10" s="50" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D12" s="82" t="s">
-        <v>104</v>
+      <c r="D12" s="50" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D13" s="82" t="s">
-        <v>105</v>
+      <c r="D13" s="50" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>